<commit_message>
Fix date comparison logic in Excel
</commit_message>
<xml_diff>
--- a/Data/dates.xlsx
+++ b/Data/dates.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\michael.agarenzo\Projects\Personal-Date-Reminder\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F5C1274-480B-416E-A68E-ECD78A0BD379}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E64057CB-09E8-42D2-B0B3-106B1FFF830F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-4344" windowWidth="30936" windowHeight="16896" xr2:uid="{E2FB14A5-F856-496F-A874-497ACF82FED6}"/>
+    <workbookView xWindow="22932" yWindow="-6792" windowWidth="30936" windowHeight="16896" xr2:uid="{E2FB14A5-F856-496F-A874-497ACF82FED6}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
@@ -441,7 +441,7 @@
   <dimension ref="A1:E100"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R14" sqref="R14"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -482,10 +482,10 @@
       </c>
       <c r="D2" s="2">
         <f ca="1">DATEDIF(C2, TODAY(), "Y")</f>
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E2" s="2" t="b">
-        <f ca="1">MONTH(C2) &amp; DAY(C2) = MONTH(TODAY()) &amp; DAY(TODAY())</f>
+        <f ca="1">TEXT(C2, "mm") &amp; TEXT(C2, "dd") = TEXT(TODAY(), "mm") &amp; TEXT(TODAY(), "dd")</f>
         <v>0</v>
       </c>
     </row>
@@ -498,7 +498,7 @@
         <v>121</v>
       </c>
       <c r="E3" s="2" t="b">
-        <f t="shared" ref="E3:E66" ca="1" si="1">MONTH(C3) &amp; DAY(C3) = MONTH(TODAY()) &amp; DAY(TODAY())</f>
+        <f t="shared" ref="E3:E66" ca="1" si="1">TEXT(C3, "mm") &amp; TEXT(C3, "dd") = TEXT(TODAY(), "mm") &amp; TEXT(TODAY(), "dd")</f>
         <v>0</v>
       </c>
     </row>
@@ -1330,7 +1330,7 @@
         <v>121</v>
       </c>
       <c r="E67" s="2" t="b">
-        <f t="shared" ref="E67:E100" ca="1" si="3">MONTH(C67) &amp; DAY(C67) = MONTH(TODAY()) &amp; DAY(TODAY())</f>
+        <f t="shared" ref="E67:E100" ca="1" si="3">TEXT(C67, "mm") &amp; TEXT(C67, "dd") = TEXT(TODAY(), "mm") &amp; TEXT(TODAY(), "dd")</f>
         <v>0</v>
       </c>
     </row>

</xml_diff>